<commit_message>
Finalisation du prototype Interprétabilité et optimisations UI
</commit_message>
<xml_diff>
--- a/Streamlit/assets/architectures/perfo_archi.xlsx
+++ b/Streamlit/assets/architectures/perfo_archi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgasm\Documents\Bernadette\IA\projet_IA\Soutenance\Images streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D235B30-109B-4DD5-8BF9-2636EAFF668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D61ED8-CFCB-4DA2-A0F0-1A3B751DF029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="6020" windowWidth="25600" windowHeight="18930" xr2:uid="{B88DEC3C-07FE-4404-A2C0-6ECB1ECD4B6B}"/>
+    <workbookView xWindow="8760" yWindow="3450" windowWidth="25600" windowHeight="18930" xr2:uid="{B88DEC3C-07FE-4404-A2C0-6ECB1ECD4B6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Nom</t>
   </si>
@@ -143,18 +143,6 @@
     <t>0.9952</t>
   </si>
   <si>
-    <t>Espèce-Macro_F1</t>
-  </si>
-  <si>
-    <t>Espèce-Accuracy</t>
-  </si>
-  <si>
-    <t>Maladie- Macro_F1</t>
-  </si>
-  <si>
-    <t>Maladie- Accuracy</t>
-  </si>
-  <si>
     <t>FLOPs (relatif)</t>
   </si>
   <si>
@@ -219,15 +207,35 @@
   </si>
   <si>
     <t>Archi</t>
+  </si>
+  <si>
+    <t>Espèce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maladie </t>
+  </si>
+  <si>
+    <t>Macro_F1</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -260,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -299,13 +307,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0070C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0070C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF0070C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF0070C0"/>
       </left>
       <right style="medium">
         <color rgb="FF0070C0"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color rgb="FF0070C0"/>
       </top>
       <bottom style="thin">
@@ -323,7 +361,7 @@
       <top style="thin">
         <color rgb="FF0070C0"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF0070C0"/>
       </bottom>
       <diagonal/>
@@ -338,7 +376,7 @@
       <top style="thin">
         <color rgb="FF0070C0"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color rgb="FF0070C0"/>
       </bottom>
       <diagonal/>
@@ -353,6 +391,19 @@
       <top style="thin">
         <color rgb="FF0070C0"/>
       </top>
+      <bottom style="medium">
+        <color rgb="FF0070C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0070C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF0070C0"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF0070C0"/>
       </bottom>
@@ -360,46 +411,46 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </left>
       <right style="medium">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF0070C0"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF0070C0"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -407,94 +458,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,377 +875,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC6B5C-2178-483E-94C3-16391CF9D80D}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7" style="8" customWidth="1"/>
-    <col min="2" max="2" width="38.7265625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" style="26" customWidth="1"/>
-    <col min="4" max="4" width="16" style="26" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" style="26" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" style="26" customWidth="1"/>
-    <col min="7" max="8" width="10.90625" style="29"/>
-    <col min="9" max="10" width="12" style="29" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="10.90625" style="8"/>
+    <col min="1" max="1" width="7" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.7265625" style="11" customWidth="1"/>
+    <col min="3" max="4" width="9.6328125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" style="18" customWidth="1"/>
+    <col min="7" max="8" width="10.90625" style="20"/>
+    <col min="9" max="9" width="12.453125" style="20" customWidth="1"/>
+    <col min="10" max="11" width="12" style="20" customWidth="1"/>
+    <col min="13" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="E2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="H2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="I2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="K2" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="11">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="E3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>55</v>
+      <c r="K3" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>53</v>
+      <c r="D4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="27" t="s">
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="28" t="s">
-        <v>56</v>
+      <c r="J5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>56</v>
+      <c r="K6" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="11">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="22">
-        <v>0.999</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="27" t="s">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="28" t="s">
-        <v>48</v>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>7</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="D8" s="14">
+        <v>0.999</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>48</v>
+      <c r="J8" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="11">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E10" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="J9" s="27" t="s">
+      <c r="G10" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="28" t="s">
-        <v>48</v>
+      <c r="J10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="19" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="12">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B11" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>57</v>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hide index column in Step 5 table and update styles
</commit_message>
<xml_diff>
--- a/Streamlit/assets/architectures/perfo_archi.xlsx
+++ b/Streamlit/assets/architectures/perfo_archi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgasm\Documents\Bernadette\IA\projet_IA\Soutenance\Images streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D61ED8-CFCB-4DA2-A0F0-1A3B751DF029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423E274C-F52C-4E85-933E-96748EA9C868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="3450" windowWidth="25600" windowHeight="18930" xr2:uid="{B88DEC3C-07FE-4404-A2C0-6ECB1ECD4B6B}"/>
+    <workbookView xWindow="12090" yWindow="1750" windowWidth="25600" windowHeight="18930" xr2:uid="{B88DEC3C-07FE-4404-A2C0-6ECB1ECD4B6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
   <si>
     <t>Nom</t>
   </si>
@@ -209,16 +209,16 @@
     <t>Archi</t>
   </si>
   <si>
-    <t>Espèce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maladie </t>
-  </si>
-  <si>
-    <t>Macro_F1</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
+    <t>Espèce-Macro_F1</t>
+  </si>
+  <si>
+    <t>Espèce-Accuracy</t>
+  </si>
+  <si>
+    <t>Maladie-Macro_F1</t>
+  </si>
+  <si>
+    <t>Maladie-Accuracy</t>
   </si>
 </sst>
 </file>
@@ -268,7 +268,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -409,56 +409,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -531,15 +486,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC6B5C-2178-483E-94C3-16391CF9D80D}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,371 +840,357 @@
     <col min="13" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C1" s="25" t="s">
+    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="E1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>38</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="D3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="19" t="s">
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="19" t="s">
+      <c r="I4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12" t="s">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="D5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>40</v>
+      <c r="I5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="19" t="s">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>54</v>
+      <c r="J6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.999</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>40</v>
+      <c r="I7" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="14" t="s">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="14">
-        <v>0.999</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="19" t="s">
+      <c r="E8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="19" t="s">
-        <v>55</v>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="12" t="s">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="E9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="14" t="s">
+    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="E10" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>